<commit_message>
Fitting on thresholds only
</commit_message>
<xml_diff>
--- a/inst/shiny_app/www/sample.xlsx
+++ b/inst/shiny_app/www/sample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="US 2010" sheetId="1" r:id="rId1"/>
+    <sheet name="File #1" sheetId="1" r:id="rId1"/>
+    <sheet name="File #2" sheetId="2" r:id="rId2"/>
+    <sheet name="File #3" sheetId="5" r:id="rId3"/>
+    <sheet name="File #4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
   <si>
     <t>year</t>
   </si>
@@ -35,6 +38,12 @@
     <t>country</t>
   </si>
   <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>popsize</t>
+  </si>
+  <si>
     <t>average</t>
   </si>
   <si>
@@ -44,10 +53,28 @@
     <t>thr</t>
   </si>
   <si>
-    <t>bracketsh</t>
-  </si>
-  <si>
-    <t>US</t>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>labor</t>
+  </si>
+  <si>
+    <t>capital</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>US1</t>
+  </si>
+  <si>
+    <t>US2</t>
   </si>
 </sst>
 </file>
@@ -362,15 +389,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,69 +416,441 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>225700000</v>
+      </c>
+      <c r="E2">
+        <v>37208</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>4130</v>
+      </c>
+      <c r="H2">
+        <v>12643</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>23686</v>
+      </c>
+      <c r="H3">
+        <v>43908</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>0.9</v>
+      </c>
+      <c r="G4">
+        <v>76252</v>
+      </c>
+      <c r="H4">
+        <v>108329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>0.99</v>
+      </c>
+      <c r="G5">
+        <v>211861</v>
+      </c>
+      <c r="H5">
+        <v>471463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>225700000</v>
+      </c>
+      <c r="E2">
+        <v>16370</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>-1176</v>
+      </c>
+      <c r="H2">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>2780</v>
+      </c>
+      <c r="H3">
+        <v>10657</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>0.9</v>
+      </c>
+      <c r="G4">
+        <v>28939</v>
+      </c>
+      <c r="H4">
+        <v>59412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>0.99</v>
+      </c>
+      <c r="G5">
+        <v>173917</v>
+      </c>
+      <c r="H5">
+        <v>688689</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>225700000</v>
+      </c>
+      <c r="E2">
         <v>53587</v>
       </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>5665</v>
+      </c>
+      <c r="H2">
+        <v>18030</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>31829</v>
+      </c>
+      <c r="H3">
+        <v>54936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>0.9</v>
+      </c>
+      <c r="G4">
+        <v>96480</v>
+      </c>
+      <c r="H4">
+        <v>151099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>0.99</v>
+      </c>
+      <c r="G5">
+        <v>351366</v>
+      </c>
+      <c r="H5">
+        <v>1068911</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>36962517</v>
       </c>
       <c r="E2">
-        <v>5665</v>
+        <v>27727</v>
       </c>
       <c r="F2">
-        <v>0.13458999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D3">
-        <v>0.5</v>
-      </c>
-      <c r="E3">
-        <v>31829</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>5387</v>
+      </c>
+      <c r="I2">
+        <v>0.872</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F3">
-        <v>0.41006999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D4">
-        <v>0.9</v>
-      </c>
-      <c r="E4">
-        <v>96480</v>
-      </c>
+        <v>0.26386999999999999</v>
+      </c>
+      <c r="G3">
+        <v>11682</v>
+      </c>
+      <c r="H3">
+        <v>12868</v>
+      </c>
+      <c r="I3">
+        <v>0.872</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F4">
-        <v>0.10537000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D5">
-        <v>0.95</v>
-      </c>
-      <c r="E5">
-        <v>136910</v>
-      </c>
+        <v>0.32899</v>
+      </c>
+      <c r="G4">
+        <v>14019</v>
+      </c>
+      <c r="H4">
+        <v>15882</v>
+      </c>
+      <c r="I4">
+        <v>0.872</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F5">
-        <v>0.1484</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D6">
-        <v>0.99</v>
-      </c>
-      <c r="E6">
-        <v>351366</v>
-      </c>
+        <v>0.43231999999999998</v>
+      </c>
+      <c r="G5">
+        <v>17523</v>
+      </c>
+      <c r="H5">
+        <v>20246</v>
+      </c>
+      <c r="I5">
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F6">
-        <v>0.19946</v>
+        <v>0.58923999999999999</v>
+      </c>
+      <c r="G6">
+        <v>23364</v>
+      </c>
+      <c r="H6">
+        <v>28735</v>
+      </c>
+      <c r="I6">
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>0.76088999999999996</v>
+      </c>
+      <c r="G7">
+        <v>35047</v>
+      </c>
+      <c r="H7">
+        <v>44451</v>
+      </c>
+      <c r="I7">
+        <v>0.26100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>0.91522000000000003</v>
+      </c>
+      <c r="G8">
+        <v>58411</v>
+      </c>
+      <c r="H8">
+        <v>76572</v>
+      </c>
+      <c r="I8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>0.98419000000000001</v>
+      </c>
+      <c r="G9">
+        <v>116822</v>
+      </c>
+      <c r="H9">
+        <v>226255</v>
+      </c>
+      <c r="I9">
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>